<commit_message>
Clean, add comments. Update final plot.
</commit_message>
<xml_diff>
--- a/inputData/Eco_GG_fixed.xlsx
+++ b/inputData/Eco_GG_fixed.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27531"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27425"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://polimi365-my.sharepoint.com/personal/10791792_polimi_it/Documents/2024-04 Economic model/EcoModel/inputData/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\PhD\GitHubRepo\EcoModel\inputData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="19" documentId="13_ncr:1_{88612981-6723-4AA0-8621-2F790BC14902}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{629917CB-6105-4846-B101-353628D22B50}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44C21C2D-7004-4215-AED6-1A226FE0C94C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="31590" yWindow="-1755" windowWidth="21600" windowHeight="11235" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="kite" sheetId="3" r:id="rId1"/>
@@ -539,13 +539,13 @@
       <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="29.1796875" customWidth="1"/>
-    <col min="2" max="2" width="17.453125" customWidth="1"/>
+    <col min="1" max="1" width="29.140625" customWidth="1"/>
+    <col min="2" max="2" width="17.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>18</v>
       </c>
@@ -553,7 +553,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -561,7 +561,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -569,7 +569,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -577,7 +577,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -585,7 +585,7 @@
         <v>3.6</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -593,7 +593,7 @@
         <v>0.75</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>25</v>
       </c>
@@ -601,7 +601,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>26</v>
       </c>
@@ -609,7 +609,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>53</v>
       </c>
@@ -617,7 +617,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>54</v>
       </c>
@@ -625,7 +625,7 @@
         <v>150000</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B14" s="1"/>
     </row>
   </sheetData>
@@ -641,13 +641,13 @@
       <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="27.81640625" customWidth="1"/>
-    <col min="2" max="2" width="23.453125" customWidth="1"/>
+    <col min="1" max="1" width="27.85546875" customWidth="1"/>
+    <col min="2" max="2" width="23.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>27</v>
       </c>
@@ -656,7 +656,7 @@
       </c>
       <c r="H1" s="1"/>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -665,7 +665,7 @@
       </c>
       <c r="H2" s="1"/>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>7</v>
       </c>
@@ -673,7 +673,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>8</v>
       </c>
@@ -681,7 +681,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>9</v>
       </c>
@@ -689,7 +689,7 @@
         <v>0.85</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>50</v>
       </c>
@@ -697,7 +697,7 @@
         <v>6.5</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>51</v>
       </c>
@@ -705,7 +705,7 @@
         <v>2.6</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>52</v>
       </c>
@@ -713,7 +713,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>55</v>
       </c>
@@ -732,24 +732,24 @@
   <dimension ref="A1:B30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+      <selection activeCell="I13" sqref="I13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="24.54296875" customWidth="1"/>
+    <col min="1" max="1" width="24.5703125" customWidth="1"/>
     <col min="2" max="2" width="11" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>10</v>
       </c>
       <c r="B1">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>11</v>
       </c>
@@ -757,7 +757,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>12</v>
       </c>
@@ -765,7 +765,7 @@
         <v>2700</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>13</v>
       </c>
@@ -774,7 +774,7 @@
         <v>300000000</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>14</v>
       </c>
@@ -782,7 +782,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>15</v>
       </c>
@@ -790,7 +790,7 @@
         <v>7850</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>16</v>
       </c>
@@ -799,7 +799,7 @@
         <v>500000000</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>45</v>
       </c>
@@ -807,7 +807,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>46</v>
       </c>
@@ -815,7 +815,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>17</v>
       </c>
@@ -823,7 +823,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>28</v>
       </c>
@@ -831,7 +831,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>29</v>
       </c>
@@ -839,7 +839,7 @@
         <v>12.9</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>30</v>
       </c>
@@ -847,7 +847,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>31</v>
       </c>
@@ -855,7 +855,7 @@
         <v>0.71</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>19</v>
       </c>
@@ -863,7 +863,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>32</v>
       </c>
@@ -871,7 +871,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>33</v>
       </c>
@@ -879,7 +879,7 @@
         <v>12.4</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>35</v>
       </c>
@@ -887,7 +887,7 @@
         <v>2.2999999999999998</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>34</v>
       </c>
@@ -895,7 +895,7 @@
         <v>3400</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>36</v>
       </c>
@@ -903,7 +903,7 @@
         <v>60000</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>37</v>
       </c>
@@ -912,7 +912,7 @@
         <v>1000000</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>38</v>
       </c>
@@ -920,7 +920,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>39</v>
       </c>
@@ -928,7 +928,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>40</v>
       </c>
@@ -936,7 +936,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>41</v>
       </c>
@@ -944,7 +944,7 @@
         <v>30000</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>42</v>
       </c>
@@ -952,7 +952,7 @@
         <v>1200</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>43</v>
       </c>
@@ -960,7 +960,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>44</v>
       </c>
@@ -968,7 +968,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>56</v>
       </c>
@@ -976,7 +976,7 @@
         <v>1.1000000000000001</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>57</v>
       </c>
@@ -998,12 +998,12 @@
       <selection activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.54296875" customWidth="1"/>
+    <col min="1" max="1" width="17.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>20</v>
       </c>
@@ -1011,7 +1011,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>21</v>
       </c>
@@ -1019,7 +1019,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>22</v>
       </c>
@@ -1027,7 +1027,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>23</v>
       </c>
@@ -1035,7 +1035,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>24</v>
       </c>
@@ -1056,7 +1056,7 @@
       <selection activeCell="D35" sqref="D35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1070,12 +1070,12 @@
       <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="27.26953125" customWidth="1"/>
+    <col min="1" max="1" width="27.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>47</v>
       </c>
@@ -1083,7 +1083,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>48</v>
       </c>
@@ -1091,7 +1091,7 @@
         <v>-1.2</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>49</v>
       </c>

</xml_diff>